<commit_message>
version 1.2 with fix
</commit_message>
<xml_diff>
--- a/WindowsFormsApp1/bin/Debug/source.xlsx
+++ b/WindowsFormsApp1/bin/Debug/source.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\project_SCADA\VS\WindowsFormsApp1\WindowsFormsApp1\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA5F0613-C69B-4524-9856-42A131CBE5D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEE4E616-DA20-42E5-AAE2-50591FC57196}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1950" yWindow="1950" windowWidth="15105" windowHeight="8850" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -994,7 +994,7 @@
     <t>became</t>
   </si>
   <si>
-    <t>12,22,18,43,6</t>
+    <t>7,27,45,37,14,30,17,50,32,42,29,46,19</t>
   </si>
 </sst>
 </file>
@@ -2792,11 +2792,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A26A3876-2E1A-4B51-B29E-34A99422CE0F}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="7"/>
+    <col min="1" max="1" width="33.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>